<commit_message>
commit requirements changes commit procfile with gunicorn creation commit debug=False in main.py changes
</commit_message>
<xml_diff>
--- a/Data/PN_threshold.xlsx
+++ b/Data/PN_threshold.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\pythonProject\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\PycharmProjects\Dashboard_final\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B3D4AB-6E58-4870-B441-B9CF09551AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A56B9A91-50D3-429B-835E-417FBFEA807F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B6CB6E03-25AF-47A0-A746-74D4A0314626}"/>
+    <workbookView xWindow="6525" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{B6CB6E03-25AF-47A0-A746-74D4A0314626}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -552,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E277A660-CA8D-4C63-BB43-576114EE5AB9}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A2:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,191 +564,177 @@
     <col min="2" max="2" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="5">
+      <c r="B2" s="5">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1">
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B3" s="5">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2">
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B4" s="5">
         <v>0.1</v>
       </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3">
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="24" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="2">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="7">
-        <v>1</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.1</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="B7" s="7">
+        <v>1</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="7">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.1</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D8">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="24" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="7">
+        <v>5</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B10" s="2">
         <v>0.3</v>
       </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9">
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10">
         <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="3">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10">
-        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="8">
-        <v>0.9</v>
+        <v>5</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
       </c>
       <c r="D11">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="8">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
       </c>
       <c r="D12">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>8</v>
-      </c>
-      <c r="B13" s="8">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="B14" s="8">
         <v>1</v>
@@ -757,26 +743,26 @@
         <v>19</v>
       </c>
       <c r="D14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="8">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>10</v>
-      </c>
-      <c r="B15" s="8">
-        <v>0.9</v>
-      </c>
-      <c r="C15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>11</v>
       </c>
       <c r="B16" s="8">
         <v>0.9</v>
@@ -785,26 +771,26 @@
         <v>19</v>
       </c>
       <c r="D16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>12</v>
-      </c>
-      <c r="B17" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="C17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="B18" s="8">
         <v>0.8</v>
@@ -813,40 +799,40 @@
         <v>19</v>
       </c>
       <c r="D18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19">
         <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="8">
-        <v>1</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19">
-        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="C20" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="D20">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="8">
         <v>0.8</v>
@@ -855,69 +841,83 @@
         <v>19</v>
       </c>
       <c r="D21">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="8">
+      <c r="B23" s="8">
         <v>1</v>
       </c>
-      <c r="C22" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22">
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23">
         <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="24" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="8">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="24" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B24" s="8">
         <v>0</v>
       </c>
       <c r="D24">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="B25" s="8">
         <v>0</v>
       </c>
       <c r="D25">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="8">
         <v>0</v>
       </c>
       <c r="D26">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="8">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>